<commit_message>
work on dental field
</commit_message>
<xml_diff>
--- a/code/dental_titles.xlsx
+++ b/code/dental_titles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Études\Ecole_Ingénieur\2A\TR-Economie\Projet_de_recherche\analysingEffectOfHealthPlanInFrance\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6762BB3D-7D1D-4D7F-838F-F6A526B67B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85E77FE-A4EE-4E7D-9BA1-00C35E585B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B2:B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -786,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -814,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -867,7 +867,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -892,7 +892,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -906,7 +906,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -962,7 +962,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -976,7 +976,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -990,7 +990,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -1001,7 +1001,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>
@@ -1012,7 +1012,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
@@ -1023,7 +1023,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>22</v>
@@ -1034,7 +1034,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>23</v>
@@ -1062,7 +1062,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1076,7 +1076,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>26</v>
@@ -1087,7 +1087,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>27</v>
@@ -1131,7 +1131,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1148,7 +1148,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
@@ -1225,7 +1225,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
         <v>34</v>
@@ -1236,7 +1236,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
         <v>35</v>
@@ -1247,7 +1247,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
         <v>36</v>
@@ -1258,7 +1258,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
         <v>37</v>
@@ -1269,7 +1269,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
         <v>38</v>
@@ -1302,7 +1302,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="s">
         <v>41</v>
@@ -1313,7 +1313,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1338,7 +1338,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
         <v>44</v>
@@ -1349,7 +1349,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1385,7 +1385,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1399,7 +1399,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1413,7 +1413,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="s">
         <v>50</v>
@@ -1435,7 +1435,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1482,7 +1482,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
         <v>56</v>
@@ -1493,7 +1493,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
         <v>57</v>
@@ -1526,7 +1526,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" t="s">
         <v>60</v>
@@ -1537,7 +1537,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" t="s">
         <v>61</v>
@@ -1592,7 +1592,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
         <v>66</v>
@@ -1603,7 +1603,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
         <v>67</v>
@@ -1614,7 +1614,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
         <v>68</v>
@@ -1625,7 +1625,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72" t="s">
         <v>69</v>
@@ -1647,7 +1647,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -1661,7 +1661,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75" t="s">
         <v>72</v>
@@ -1672,7 +1672,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" t="s">
         <v>73</v>
@@ -1683,7 +1683,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="s">
         <v>74</v>
@@ -1694,7 +1694,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" t="s">
         <v>75</v>
@@ -1716,7 +1716,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" t="s">
         <v>77</v>
@@ -1727,7 +1727,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" t="s">
         <v>78</v>
@@ -1749,7 +1749,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" t="s">
         <v>80</v>
@@ -1760,7 +1760,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84" t="s">
         <v>81</v>
@@ -1782,7 +1782,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" t="s">
         <v>83</v>
@@ -1793,7 +1793,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87" t="s">
         <v>84</v>
@@ -1804,7 +1804,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E88" t="s">
         <v>85</v>
@@ -1837,7 +1837,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91" t="s">
         <v>88</v>
@@ -1848,7 +1848,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" t="s">
         <v>89</v>
@@ -1859,7 +1859,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93" t="s">
         <v>90</v>
@@ -1892,7 +1892,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -1909,7 +1909,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -1926,7 +1926,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -1943,7 +1943,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99" t="s">
         <v>96</v>
@@ -1954,7 +1954,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" t="s">
         <v>97</v>
@@ -1965,7 +1965,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -1993,7 +1993,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" t="s">
         <v>100</v>
@@ -2004,7 +2004,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104" t="s">
         <v>101</v>
@@ -2015,7 +2015,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" t="s">
         <v>102</v>
@@ -2026,7 +2026,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" t="s">
         <v>103</v>
@@ -2037,7 +2037,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" t="s">
         <v>104</v>
@@ -2048,7 +2048,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" t="s">
         <v>105</v>
@@ -2059,7 +2059,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" t="s">
         <v>106</v>
@@ -2070,7 +2070,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" t="s">
         <v>107</v>
@@ -2081,7 +2081,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" t="s">
         <v>108</v>
@@ -2092,7 +2092,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" t="s">
         <v>109</v>
@@ -2103,7 +2103,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" t="s">
         <v>110</v>
@@ -2114,7 +2114,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E114" t="s">
         <v>111</v>
@@ -2125,7 +2125,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E115" t="s">
         <v>112</v>
@@ -2136,7 +2136,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -2201,10 +2201,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2671075-8E2B-458A-B242-6A5FB3C659BE}">
-  <dimension ref="B1:B117"/>
+  <dimension ref="B1:B120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B117"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
@@ -2336,7 +2336,7 @@
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.35">
@@ -2356,12 +2356,12 @@
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.35">
@@ -2596,7 +2596,7 @@
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
@@ -2611,7 +2611,7 @@
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.35">
@@ -2626,7 +2626,7 @@
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.35">
@@ -2646,12 +2646,12 @@
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.35">
@@ -2671,12 +2671,12 @@
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.35">
@@ -2711,72 +2711,72 @@
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B111">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.35">
@@ -2791,6 +2791,21 @@
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B120">
         <v>1</v>
       </c>
     </row>

</xml_diff>